<commit_message>
feat: read ng_db.xlsx, install xlsx plugin and create xlsx-to-json.js
</commit_message>
<xml_diff>
--- a/src/db/ng_db.xlsx
+++ b/src/db/ng_db.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -83,9 +83,6 @@
     <t>А1</t>
   </si>
   <si>
-    <t>А4</t>
-  </si>
-  <si>
     <t>2619.9</t>
   </si>
   <si>
@@ -111,6 +108,24 @@
   </si>
   <si>
     <t>А</t>
+  </si>
+  <si>
+    <t>2-этажное Здание АБК (1-очередь)  пл. 589,18 м2, 000000032</t>
+  </si>
+  <si>
+    <t>3-этажное Здание АБК  (2-я очередь), Ново-Гайвинская, 92 566,1 м2 инв.№117, 00-000007</t>
+  </si>
+  <si>
+    <t>А2</t>
+  </si>
+  <si>
+    <t>А3</t>
+  </si>
+  <si>
+    <t>566.1</t>
+  </si>
+  <si>
+    <t>589.18</t>
   </si>
 </sst>
 </file>
@@ -438,7 +453,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -510,10 +525,10 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -521,7 +536,7 @@
         <v>2012</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -539,14 +554,14 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -554,42 +569,54 @@
         <v>2014</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1">
+        <v>117</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>

</xml_diff>

<commit_message>
feat: modify xlsx-to-json.js and ng_db.xlsx
</commit_message>
<xml_diff>
--- a/src/db/ng_db.xlsx
+++ b/src/db/ng_db.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svv\Desktop\web-projects\ingc-map\src\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvsh\Desktop\web-projects\ingc-map\src\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F618181-308D-4847-90ED-64DFEA5E604F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23625" windowHeight="12180"/>
+    <workbookView xWindow="32325" yWindow="1395" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -65,15 +66,9 @@
     <t>ceh1</t>
   </si>
   <si>
-    <t>Цех производственный №1</t>
-  </si>
-  <si>
     <t>ceh2</t>
   </si>
   <si>
-    <t>Цех производственный №2</t>
-  </si>
-  <si>
     <t>Производственная база по механической сборке метал. конструкций, Ново-Гайв, 92 1оч пл.2663,19, 000000034</t>
   </si>
   <si>
@@ -89,9 +84,6 @@
     <t>2663.19</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>ул. Ново-Гайвинская, 92</t>
   </si>
   <si>
@@ -126,12 +118,30 @@
   </si>
   <si>
     <t>589.18</t>
+  </si>
+  <si>
+    <t>Цех (I очередь)</t>
+  </si>
+  <si>
+    <t>Цех (II очередь)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>59:01:2910297:172</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,17 +459,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
@@ -468,7 +478,7 @@
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,123 +516,189 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2663.19</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="L2" s="1">
         <v>2012</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>116</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="L3" s="1">
         <v>2014</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2012</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D5" s="1">
         <v>117</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2014</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -636,7 +712,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -650,7 +726,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -664,7 +740,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -678,7 +754,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -692,7 +768,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -706,7 +782,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -720,7 +796,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -734,7 +810,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -748,7 +824,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -762,7 +838,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -931,172 +1007,46 @@
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>